<commit_message>
Resolved merge conflicts and integrated remote changes
</commit_message>
<xml_diff>
--- a/Dieta.xlsx
+++ b/Dieta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/79f1909e597772fb/Dieta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/79f1909e597772fb/Dieta/dist/Dieta Github/Diet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="959" documentId="8_{90986033-560C-486B-8143-87D885832CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DF1E34E-7DD2-4794-B0CA-E397F0F302B9}"/>
+  <xr:revisionPtr revIDLastSave="960" documentId="8_{90986033-560C-486B-8143-87D885832CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0555D498-A03E-42C4-A68D-D63D1EFDAB1D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EEAF446F-95DF-4CB5-9D66-62E4FEDCD420}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
   <si>
     <t>Pão Integral</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>60g Morango | 60g Melão | 35g Uva</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -1194,12 +1197,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1237,27 +1261,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1597,8 +1600,8 @@
   <dimension ref="A1:T106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102:L102"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P105" sqref="P105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,11 +1622,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
       <c r="D1" s="21" t="s">
         <v>43</v>
       </c>
@@ -1638,7 +1641,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1662,7 +1665,7 @@
       <c r="H2" s="59"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
+      <c r="A3" s="69"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1683,7 +1686,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="64"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1704,7 +1707,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="64"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1741,7 +1744,7 @@
       <c r="H7" s="60"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="69" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1762,7 +1765,7 @@
       <c r="G8" s="55">
         <v>89</v>
       </c>
-      <c r="N8" s="65"/>
+      <c r="N8" s="72"/>
       <c r="P8" s="28"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1770,7 +1773,7 @@
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1789,7 +1792,7 @@
       <c r="G9" s="16">
         <v>51</v>
       </c>
-      <c r="N9" s="65"/>
+      <c r="N9" s="72"/>
       <c r="P9" s="28"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1825,7 +1828,7 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="69" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1855,7 +1858,7 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="2" t="s">
         <v>50</v>
       </c>
@@ -1883,7 +1886,7 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1982,7 +1985,7 @@
       <c r="H19" s="60"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="69" t="s">
         <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2008,7 +2011,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
+      <c r="A21" s="69"/>
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
@@ -2032,7 +2035,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
@@ -2075,7 +2078,7 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="69" t="s">
         <v>60</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2105,7 +2108,7 @@
       <c r="T25" s="1"/>
     </row>
     <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
+      <c r="A26" s="69"/>
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
@@ -2159,7 +2162,7 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="69" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2186,7 +2189,7 @@
       <c r="T29" s="1"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="64"/>
+      <c r="A30" s="69"/>
       <c r="B30" s="2" t="s">
         <v>19</v>
       </c>
@@ -2211,7 +2214,7 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="64"/>
+      <c r="A31" s="69"/>
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -2281,11 +2284,11 @@
       <c r="T37" s="1"/>
     </row>
     <row r="38" spans="1:20" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="77"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="84"/>
       <c r="N38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -2300,7 +2303,7 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="72" t="s">
+      <c r="A40" s="79" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2331,7 +2334,7 @@
       <c r="T40" s="1"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="73"/>
+      <c r="A41" s="80"/>
       <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
@@ -2361,7 +2364,7 @@
       <c r="T41" s="1"/>
     </row>
     <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="74"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="2" t="s">
         <v>16</v>
       </c>
@@ -2417,7 +2420,7 @@
     </row>
     <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="69" t="s">
         <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2444,7 +2447,7 @@
       <c r="L46" s="58"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="72"/>
+      <c r="A47" s="79"/>
       <c r="B47" s="2" t="s">
         <v>2</v>
       </c>
@@ -2470,7 +2473,7 @@
       <c r="L47" s="28"/>
     </row>
     <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="72"/>
+      <c r="A48" s="79"/>
       <c r="B48" s="2" t="s">
         <v>16</v>
       </c>
@@ -2512,7 +2515,7 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="72" t="s">
+      <c r="A52" s="79" t="s">
         <v>64</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2539,7 +2542,7 @@
       <c r="L52" s="58"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="73"/>
+      <c r="A53" s="80"/>
       <c r="B53" s="5" t="s">
         <v>8</v>
       </c>
@@ -2565,7 +2568,7 @@
       <c r="L53" s="28"/>
     </row>
     <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="74"/>
+      <c r="A54" s="81"/>
       <c r="B54" s="5" t="s">
         <v>41</v>
       </c>
@@ -2607,7 +2610,7 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="64" t="s">
+      <c r="A58" s="69" t="s">
         <v>65</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -2634,7 +2637,7 @@
       <c r="L58" s="58"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="64"/>
+      <c r="A59" s="69"/>
       <c r="B59" s="2" t="s">
         <v>29</v>
       </c>
@@ -2660,7 +2663,7 @@
       <c r="L59" s="28"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="64"/>
+      <c r="A60" s="69"/>
       <c r="B60" s="2" t="s">
         <v>30</v>
       </c>
@@ -2701,13 +2704,13 @@
       <c r="L62" s="26"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="64" t="s">
+      <c r="A64" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="66" t="s">
+      <c r="B64" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="C64" s="69">
+      <c r="C64" s="76">
         <v>2</v>
       </c>
       <c r="I64" s="58"/>
@@ -2716,9 +2719,9 @@
       <c r="L64" s="58"/>
     </row>
     <row r="65" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="64"/>
-      <c r="B65" s="67"/>
-      <c r="C65" s="70"/>
+      <c r="A65" s="69"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="77"/>
       <c r="D65" s="42">
         <v>11.2</v>
       </c>
@@ -2738,9 +2741,9 @@
       <c r="L65" s="28"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="64"/>
-      <c r="B66" s="68"/>
-      <c r="C66" s="71"/>
+      <c r="A66" s="69"/>
+      <c r="B66" s="75"/>
+      <c r="C66" s="78"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -2762,7 +2765,7 @@
     </row>
     <row r="69" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="63" t="s">
+      <c r="A70" s="71" t="s">
         <v>67</v>
       </c>
       <c r="B70" s="30" t="s">
@@ -2789,7 +2792,7 @@
       <c r="L70" s="58"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="63"/>
+      <c r="A71" s="71"/>
       <c r="B71" s="30" t="s">
         <v>54</v>
       </c>
@@ -2817,7 +2820,7 @@
       <c r="L71" s="28"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="63"/>
+      <c r="A72" s="71"/>
       <c r="B72" s="30" t="s">
         <v>2</v>
       </c>
@@ -2860,7 +2863,7 @@
     </row>
     <row r="75" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="64" t="s">
+      <c r="A76" s="69" t="s">
         <v>70</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -2883,7 +2886,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="64"/>
+      <c r="A77" s="69"/>
       <c r="B77" s="2" t="s">
         <v>34</v>
       </c>
@@ -2904,7 +2907,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="64"/>
+      <c r="A78" s="69"/>
       <c r="B78" s="2" t="s">
         <v>35</v>
       </c>
@@ -2944,7 +2947,7 @@
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="82" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="64" t="s">
+      <c r="A82" s="69" t="s">
         <v>68</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -2967,7 +2970,7 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="64"/>
+      <c r="A83" s="69"/>
       <c r="B83" s="2" t="s">
         <v>19</v>
       </c>
@@ -2988,7 +2991,7 @@
       </c>
     </row>
     <row r="84" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="64"/>
+      <c r="A84" s="69"/>
       <c r="B84" s="2" t="s">
         <v>39</v>
       </c>
@@ -3028,7 +3031,7 @@
     </row>
     <row r="87" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="72" t="s">
+      <c r="A88" s="79" t="s">
         <v>69</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -3051,7 +3054,7 @@
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="73"/>
+      <c r="A89" s="80"/>
       <c r="B89" s="2" t="s">
         <v>19</v>
       </c>
@@ -3072,7 +3075,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="74"/>
+      <c r="A90" s="81"/>
       <c r="B90" s="2" t="s">
         <v>41</v>
       </c>
@@ -3109,7 +3112,7 @@
     </row>
     <row r="93" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="64" t="s">
+      <c r="A94" s="69" t="s">
         <v>74</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -3132,7 +3135,7 @@
       </c>
     </row>
     <row r="95" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="64"/>
+      <c r="A95" s="69"/>
       <c r="B95" s="2" t="s">
         <v>73</v>
       </c>
@@ -3156,7 +3159,7 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="25"/>
       <c r="B97" s="26"/>
       <c r="C97" s="25"/>
@@ -3170,9 +3173,9 @@
       <c r="K97" s="26"/>
       <c r="L97" s="26"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="99" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="64" t="s">
+    <row r="98" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="69" t="s">
         <v>79</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -3194,8 +3197,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="64"/>
+    <row r="100" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="69"/>
       <c r="B100" s="2" t="s">
         <v>50</v>
       </c>
@@ -3215,8 +3218,8 @@
         <v>293</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="25"/>
       <c r="B102" s="26"/>
       <c r="C102" s="25"/>
@@ -3230,9 +3233,9 @@
       <c r="K102" s="26"/>
       <c r="L102" s="26"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="63" t="s">
+    <row r="103" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="71" t="s">
         <v>81</v>
       </c>
       <c r="B104" s="30" t="s">
@@ -3241,50 +3244,46 @@
       <c r="C104" s="31">
         <v>1</v>
       </c>
-      <c r="D104" s="79">
+      <c r="D104" s="63">
         <v>1.9</v>
       </c>
-      <c r="E104" s="80">
+      <c r="E104" s="64">
         <v>21</v>
       </c>
-      <c r="F104" s="80">
+      <c r="F104" s="64">
         <v>5.5</v>
       </c>
-      <c r="G104" s="81">
+      <c r="G104" s="65">
         <v>123</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="63"/>
+    <row r="105" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="71"/>
       <c r="B105" s="30" t="s">
         <v>16</v>
       </c>
       <c r="C105" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D105" s="82">
+      <c r="D105" s="66">
         <v>1.78</v>
       </c>
-      <c r="E105" s="83">
+      <c r="E105" s="67">
         <v>0</v>
       </c>
-      <c r="F105" s="83">
+      <c r="F105" s="67">
         <v>15.51</v>
       </c>
-      <c r="G105" s="84">
+      <c r="G105" s="68">
         <v>82</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="P105" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A104:A105"/>
     <mergeCell ref="A99:A100"/>
     <mergeCell ref="N8:N9"/>
@@ -3301,6 +3300,13 @@
     <mergeCell ref="A70:A72"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>